<commit_message>
Updates for NuGet, Pipenv, CMake, autoconf
</commit_message>
<xml_diff>
--- a/Evaluation Framework for Dependency Analysis.xlsx
+++ b/Evaluation Framework for Dependency Analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/eclipse-workspace/efda/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/darius/workspace/efda/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C46C27D-E2C9-094D-99FD-0D615C1C33F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA3D22A-7476-0848-91B1-1DEF9FFDF686}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="33600" windowHeight="19220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6900" yWindow="5160" windowWidth="33600" windowHeight="19220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EFDA framework" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="90">
   <si>
     <t>Languages</t>
   </si>
@@ -255,13 +255,49 @@
   </si>
   <si>
     <t>EAR</t>
+  </si>
+  <si>
+    <t>C/C++</t>
+  </si>
+  <si>
+    <t>Makefile</t>
+  </si>
+  <si>
+    <t>Vendored dependecies</t>
+  </si>
+  <si>
+    <t>System dependencies</t>
+  </si>
+  <si>
+    <t>autoconf</t>
+  </si>
+  <si>
+    <t>Pipenv</t>
+  </si>
+  <si>
+    <t>With Pipfile.lock</t>
+  </si>
+  <si>
+    <t>.NET</t>
+  </si>
+  <si>
+    <t>NuGet</t>
+  </si>
+  <si>
+    <t>PackageReference</t>
+  </si>
+  <si>
+    <t>packages.config</t>
+  </si>
+  <si>
+    <t>CMake</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -271,22 +307,32 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -299,7 +345,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -309,53 +355,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -363,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -373,43 +382,54 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -724,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1006"/>
+  <dimension ref="A1:I1013"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52:B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -773,806 +793,931 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="5">
-        <f t="shared" ref="I2:I46" si="0">SUM(E2:H2)*D2</f>
+      <c r="D2" s="9"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="8">
+        <f t="shared" ref="I2:I47" si="0">SUM(E2:H2)*D2</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="5" t="s">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="5">
+      <c r="D3" s="9"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="5" t="s">
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="5">
+      <c r="D4" s="9"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="5" t="s">
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="5">
+      <c r="D5" s="9"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="5" t="s">
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="5">
+      <c r="D6" s="9"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="5" t="s">
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="5">
+      <c r="D7" s="9"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="14"/>
-      <c r="B8" s="13" t="s">
+      <c r="A8" s="23"/>
+      <c r="B8" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="5">
+      <c r="D8" s="9"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="14"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="5" t="s">
+      <c r="A9" s="23"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="5">
+      <c r="D9" s="9"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="14"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="5" t="s">
+      <c r="A10" s="23"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="5">
+      <c r="D10" s="9"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="14"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="20" t="s">
+      <c r="A11" s="23"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="5"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="14"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="20" t="s">
+      <c r="A12" s="23"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="5"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="14"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="20" t="s">
+      <c r="A13" s="23"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="5"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="14"/>
-      <c r="B14" s="13" t="s">
+      <c r="A14" s="23"/>
+      <c r="B14" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="5">
+      <c r="D14" s="9"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="14"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="8" t="s">
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="5">
+      <c r="D15" s="9"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="14"/>
-      <c r="B16" s="13" t="s">
+      <c r="A16" s="23"/>
+      <c r="B16" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="5">
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="5" t="s">
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="5">
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="5" t="s">
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="5">
-        <f t="shared" si="0"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="23"/>
+      <c r="B20" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B21" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C21" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="14"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="5" t="s">
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="23"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="14"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="9" t="s">
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="23"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="14"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="5" t="s">
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="23"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="14"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="20" t="s">
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="23"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="5"/>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="14"/>
-      <c r="B25" s="13" t="s">
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="23"/>
+      <c r="B26" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C26" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="14"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="20" t="s">
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="23"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="5"/>
-    </row>
-    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="14"/>
-      <c r="B27" s="13" t="s">
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="23"/>
+      <c r="B28" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C28" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="5" t="s">
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="23"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="13" t="s">
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B30" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C30" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="5" t="s">
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="23"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="5" t="s">
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="23"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="13" t="s">
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B33" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C33" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="15"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="5" t="s">
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="23"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="13" t="s">
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B35" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C35" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="5" t="s">
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="23"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="5" t="s">
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="23"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="13" t="s">
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B38" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C38" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="14"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="5" t="s">
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="23"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="14"/>
-      <c r="B39" s="10" t="s">
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="23"/>
+      <c r="B40" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C40" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="14"/>
-      <c r="B40" s="10" t="s">
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="23"/>
+      <c r="B41" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C41" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="14"/>
-      <c r="B41" s="10" t="s">
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="23"/>
+      <c r="B42" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C42" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="14"/>
-      <c r="B42" s="22" t="s">
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="23"/>
+      <c r="B43" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="C42" s="20" t="s">
+      <c r="C43" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="5"/>
-    </row>
-    <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="15"/>
-      <c r="B43" s="11" t="s">
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="23"/>
+      <c r="B44" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="C44" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="13" t="s">
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B44" s="13" t="s">
+      <c r="B45" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C45" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="14"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="5" t="s">
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="23"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="15"/>
-      <c r="B46" s="15"/>
-      <c r="C46" s="5" t="s">
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="23"/>
+      <c r="B47" s="23"/>
+      <c r="C47" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="H47" s="12" t="s">
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B48" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="22"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+      <c r="I49" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="22"/>
+      <c r="B51" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="22"/>
+      <c r="B52" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="22"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C54" s="7"/>
+      <c r="H54" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="I47">
-        <f>SUM(I2:I46)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="H48" s="12" t="s">
+      <c r="I54">
+        <f>SUM(I2:I53)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H55" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="I48">
-        <f>4*SUM(D2:D46)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="H49" s="12" t="s">
+      <c r="I55">
+        <f>4*SUM(D2:D53)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H56" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I49">
-        <f>ROUND(IF(I48=0,0,I47/I48), 4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="51" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="H51" s="16" t="s">
+      <c r="I56">
+        <f>ROUND(IF(I55=0,0,I54/I55), 4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="58" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H58" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="I51" s="17"/>
-    </row>
-    <row r="52" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="53" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="54" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="55" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="56" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="57" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="58" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="59" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="60" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="61" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="62" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="63" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="64" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+      <c r="I58" s="25"/>
+    </row>
+    <row r="59" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="60" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="61" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="62" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="63" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="64" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2515,36 +2660,47 @@
     <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="1006" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1007" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1008" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1009" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1010" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1011" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1012" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1013" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="26">
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="B14:B15"/>
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="A20:A28"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="A21:A29"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="B28:B29"/>
     <mergeCell ref="B8:B13"/>
-    <mergeCell ref="B20:B24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A50:A53"/>
     <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A37:A43"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A38:A44"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B45:B47"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select 0 (false) or 1 (true)" sqref="E2:H46" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select 0 (false) or 1 (true)" sqref="E2:H50" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"0.0,1.0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="D2:D46" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="D2:D50" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"0.0,1.0,2.0,3.0,4.0,5.0"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2554,10 +2710,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I1006"/>
+  <dimension ref="A1:I1013"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52:B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2603,1274 +2759,1463 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="9">
         <v>5</v>
       </c>
-      <c r="E2" s="7">
-        <v>1</v>
-      </c>
-      <c r="F2" s="7">
-        <v>1</v>
-      </c>
-      <c r="G2" s="7">
-        <v>1</v>
-      </c>
-      <c r="H2" s="7">
-        <v>1</v>
-      </c>
-      <c r="I2" s="5">
-        <f t="shared" ref="I2:I46" si="0">SUM(E2:H2)*D2</f>
+      <c r="E2" s="15">
+        <v>1</v>
+      </c>
+      <c r="F2" s="15">
+        <v>1</v>
+      </c>
+      <c r="G2" s="15">
+        <v>1</v>
+      </c>
+      <c r="H2" s="15">
+        <v>1</v>
+      </c>
+      <c r="I2" s="8">
+        <f t="shared" ref="I2:I53" si="0">SUM(E2:H2)*D2</f>
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="5" t="s">
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="9">
         <v>5</v>
       </c>
-      <c r="E3" s="7">
-        <v>1</v>
-      </c>
-      <c r="F3" s="7">
-        <v>1</v>
-      </c>
-      <c r="G3" s="7">
-        <v>1</v>
-      </c>
-      <c r="H3" s="7">
-        <v>1</v>
-      </c>
-      <c r="I3" s="5">
+      <c r="E3" s="15">
+        <v>1</v>
+      </c>
+      <c r="F3" s="15">
+        <v>1</v>
+      </c>
+      <c r="G3" s="15">
+        <v>1</v>
+      </c>
+      <c r="H3" s="15">
+        <v>1</v>
+      </c>
+      <c r="I3" s="8">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="5" t="s">
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="9">
         <v>5</v>
       </c>
-      <c r="E4" s="7">
-        <v>1</v>
-      </c>
-      <c r="F4" s="7">
-        <v>1</v>
-      </c>
-      <c r="G4" s="7">
-        <v>1</v>
-      </c>
-      <c r="H4" s="7">
-        <v>1</v>
-      </c>
-      <c r="I4" s="5">
+      <c r="E4" s="15">
+        <v>1</v>
+      </c>
+      <c r="F4" s="15">
+        <v>1</v>
+      </c>
+      <c r="G4" s="15">
+        <v>1</v>
+      </c>
+      <c r="H4" s="15">
+        <v>1</v>
+      </c>
+      <c r="I4" s="8">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="5" t="s">
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="9">
         <v>5</v>
       </c>
-      <c r="E5" s="7">
-        <v>1</v>
-      </c>
-      <c r="F5" s="7">
-        <v>1</v>
-      </c>
-      <c r="G5" s="7">
-        <v>1</v>
-      </c>
-      <c r="H5" s="7">
-        <v>1</v>
-      </c>
-      <c r="I5" s="5">
+      <c r="E5" s="15">
+        <v>1</v>
+      </c>
+      <c r="F5" s="15">
+        <v>1</v>
+      </c>
+      <c r="G5" s="15">
+        <v>1</v>
+      </c>
+      <c r="H5" s="15">
+        <v>1</v>
+      </c>
+      <c r="I5" s="8">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="5" t="s">
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="7">
-        <v>1</v>
-      </c>
-      <c r="F6" s="7">
-        <v>1</v>
-      </c>
-      <c r="G6" s="7">
-        <v>1</v>
-      </c>
-      <c r="H6" s="7">
-        <v>1</v>
-      </c>
-      <c r="I6" s="5">
+      <c r="D6" s="9">
+        <v>0</v>
+      </c>
+      <c r="E6" s="15">
+        <v>1</v>
+      </c>
+      <c r="F6" s="15">
+        <v>1</v>
+      </c>
+      <c r="G6" s="15">
+        <v>1</v>
+      </c>
+      <c r="H6" s="15">
+        <v>1</v>
+      </c>
+      <c r="I6" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="5" t="s">
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="6">
-        <v>0</v>
-      </c>
-      <c r="E7" s="7">
-        <v>1</v>
-      </c>
-      <c r="F7" s="7">
-        <v>1</v>
-      </c>
-      <c r="G7" s="7">
-        <v>1</v>
-      </c>
-      <c r="H7" s="7">
-        <v>1</v>
-      </c>
-      <c r="I7" s="5">
+      <c r="D7" s="9">
+        <v>0</v>
+      </c>
+      <c r="E7" s="15">
+        <v>1</v>
+      </c>
+      <c r="F7" s="15">
+        <v>1</v>
+      </c>
+      <c r="G7" s="15">
+        <v>1</v>
+      </c>
+      <c r="H7" s="15">
+        <v>1</v>
+      </c>
+      <c r="I7" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="14"/>
-      <c r="B8" s="13" t="s">
+      <c r="A8" s="22"/>
+      <c r="B8" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="9">
         <v>5</v>
       </c>
-      <c r="E8" s="7">
-        <v>1</v>
-      </c>
-      <c r="F8" s="7">
-        <v>0</v>
-      </c>
-      <c r="G8" s="7">
-        <v>1</v>
-      </c>
-      <c r="H8" s="7">
-        <v>0</v>
-      </c>
-      <c r="I8" s="5">
+      <c r="E8" s="15">
+        <v>1</v>
+      </c>
+      <c r="F8" s="15">
+        <v>0</v>
+      </c>
+      <c r="G8" s="15">
+        <v>1</v>
+      </c>
+      <c r="H8" s="15">
+        <v>0</v>
+      </c>
+      <c r="I8" s="8">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="14"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="5" t="s">
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="6">
-        <v>0</v>
-      </c>
-      <c r="E9" s="7">
-        <v>1</v>
-      </c>
-      <c r="F9" s="7">
-        <v>0</v>
-      </c>
-      <c r="G9" s="7">
-        <v>1</v>
-      </c>
-      <c r="H9" s="7">
-        <v>0</v>
-      </c>
-      <c r="I9" s="5">
+      <c r="D9" s="9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="15">
+        <v>1</v>
+      </c>
+      <c r="F9" s="15">
+        <v>0</v>
+      </c>
+      <c r="G9" s="15">
+        <v>1</v>
+      </c>
+      <c r="H9" s="15">
+        <v>0</v>
+      </c>
+      <c r="I9" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="14"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="5" t="s">
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="6">
-        <v>0</v>
-      </c>
-      <c r="E10" s="7">
-        <v>1</v>
-      </c>
-      <c r="F10" s="7">
-        <v>0</v>
-      </c>
-      <c r="G10" s="7">
-        <v>1</v>
-      </c>
-      <c r="H10" s="7">
-        <v>0</v>
-      </c>
-      <c r="I10" s="5">
+      <c r="D10" s="9">
+        <v>0</v>
+      </c>
+      <c r="E10" s="15">
+        <v>1</v>
+      </c>
+      <c r="F10" s="15">
+        <v>0</v>
+      </c>
+      <c r="G10" s="15">
+        <v>1</v>
+      </c>
+      <c r="H10" s="15">
+        <v>0</v>
+      </c>
+      <c r="I10" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="14"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="20" t="s">
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="6">
-        <v>0</v>
-      </c>
-      <c r="E11" s="7">
-        <v>1</v>
-      </c>
-      <c r="F11" s="7">
-        <v>1</v>
-      </c>
-      <c r="G11" s="7">
-        <v>0</v>
-      </c>
-      <c r="H11" s="7">
-        <v>0</v>
-      </c>
-      <c r="I11" s="5">
+      <c r="D11" s="9">
+        <v>0</v>
+      </c>
+      <c r="E11" s="15">
+        <v>1</v>
+      </c>
+      <c r="F11" s="15">
+        <v>1</v>
+      </c>
+      <c r="G11" s="15">
+        <v>0</v>
+      </c>
+      <c r="H11" s="15">
+        <v>0</v>
+      </c>
+      <c r="I11" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="14"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="20" t="s">
+      <c r="A12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="D12" s="6">
-        <v>0</v>
-      </c>
-      <c r="E12" s="7">
-        <v>1</v>
-      </c>
-      <c r="F12" s="7">
-        <v>1</v>
-      </c>
-      <c r="G12" s="7">
-        <v>0</v>
-      </c>
-      <c r="H12" s="7">
-        <v>0</v>
-      </c>
-      <c r="I12" s="5">
+      <c r="D12" s="9">
+        <v>0</v>
+      </c>
+      <c r="E12" s="15">
+        <v>1</v>
+      </c>
+      <c r="F12" s="15">
+        <v>1</v>
+      </c>
+      <c r="G12" s="15">
+        <v>0</v>
+      </c>
+      <c r="H12" s="15">
+        <v>0</v>
+      </c>
+      <c r="I12" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="14"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="20" t="s">
+      <c r="A13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="D13" s="6">
-        <v>0</v>
-      </c>
-      <c r="E13" s="7">
-        <v>1</v>
-      </c>
-      <c r="F13" s="7">
-        <v>1</v>
-      </c>
-      <c r="G13" s="7">
-        <v>0</v>
-      </c>
-      <c r="H13" s="7">
-        <v>0</v>
-      </c>
-      <c r="I13" s="5">
+      <c r="D13" s="9">
+        <v>0</v>
+      </c>
+      <c r="E13" s="15">
+        <v>1</v>
+      </c>
+      <c r="F13" s="15">
+        <v>1</v>
+      </c>
+      <c r="G13" s="15">
+        <v>0</v>
+      </c>
+      <c r="H13" s="15">
+        <v>0</v>
+      </c>
+      <c r="I13" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="14"/>
-      <c r="B14" s="13" t="s">
+      <c r="A14" s="22"/>
+      <c r="B14" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="9">
         <v>5</v>
       </c>
-      <c r="E14" s="7">
-        <v>1</v>
-      </c>
-      <c r="F14" s="7">
-        <v>1</v>
-      </c>
-      <c r="G14" s="7">
-        <v>1</v>
-      </c>
-      <c r="H14" s="7">
-        <v>1</v>
-      </c>
-      <c r="I14" s="5">
+      <c r="E14" s="15">
+        <v>1</v>
+      </c>
+      <c r="F14" s="15">
+        <v>1</v>
+      </c>
+      <c r="G14" s="15">
+        <v>1</v>
+      </c>
+      <c r="H14" s="15">
+        <v>1</v>
+      </c>
+      <c r="I14" s="8">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="14"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="8" t="s">
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="9">
         <v>5</v>
       </c>
-      <c r="E15" s="7">
-        <v>1</v>
-      </c>
-      <c r="F15" s="7">
-        <v>0</v>
-      </c>
-      <c r="G15" s="7">
-        <v>1</v>
-      </c>
-      <c r="H15" s="7">
-        <v>1</v>
-      </c>
-      <c r="I15" s="5">
+      <c r="E15" s="15">
+        <v>1</v>
+      </c>
+      <c r="F15" s="15">
+        <v>0</v>
+      </c>
+      <c r="G15" s="15">
+        <v>1</v>
+      </c>
+      <c r="H15" s="15">
+        <v>1</v>
+      </c>
+      <c r="I15" s="8">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="14"/>
-      <c r="B16" s="13" t="s">
+      <c r="A16" s="22"/>
+      <c r="B16" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="9">
         <v>5</v>
       </c>
-      <c r="E16" s="7">
-        <v>1</v>
-      </c>
-      <c r="F16" s="7">
-        <v>1</v>
-      </c>
-      <c r="G16" s="7">
-        <v>1</v>
-      </c>
-      <c r="H16" s="7">
-        <v>1</v>
-      </c>
-      <c r="I16" s="5">
+      <c r="E16" s="15">
+        <v>1</v>
+      </c>
+      <c r="F16" s="15">
+        <v>1</v>
+      </c>
+      <c r="G16" s="15">
+        <v>1</v>
+      </c>
+      <c r="H16" s="15">
+        <v>1</v>
+      </c>
+      <c r="I16" s="8">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="5" t="s">
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="9">
         <v>3</v>
       </c>
-      <c r="E17" s="7">
-        <v>1</v>
-      </c>
-      <c r="F17" s="7">
-        <v>1</v>
-      </c>
-      <c r="G17" s="7">
-        <v>1</v>
-      </c>
-      <c r="H17" s="7">
-        <v>1</v>
-      </c>
-      <c r="I17" s="5">
+      <c r="E17" s="15">
+        <v>1</v>
+      </c>
+      <c r="F17" s="15">
+        <v>1</v>
+      </c>
+      <c r="G17" s="15">
+        <v>1</v>
+      </c>
+      <c r="H17" s="15">
+        <v>1</v>
+      </c>
+      <c r="I17" s="8">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="9">
         <v>3</v>
       </c>
-      <c r="E18" s="7">
-        <v>1</v>
-      </c>
-      <c r="F18" s="7">
-        <v>1</v>
-      </c>
-      <c r="G18" s="7">
-        <v>1</v>
-      </c>
-      <c r="H18" s="7">
-        <v>1</v>
-      </c>
-      <c r="I18" s="5">
+      <c r="E18" s="15">
+        <v>1</v>
+      </c>
+      <c r="F18" s="15">
+        <v>1</v>
+      </c>
+      <c r="G18" s="15">
+        <v>1</v>
+      </c>
+      <c r="H18" s="15">
+        <v>1</v>
+      </c>
+      <c r="I18" s="8">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="5" t="s">
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="6">
-        <v>0</v>
-      </c>
-      <c r="E19" s="7">
-        <v>1</v>
-      </c>
-      <c r="F19" s="7">
-        <v>1</v>
-      </c>
-      <c r="G19" s="7">
-        <v>1</v>
-      </c>
-      <c r="H19" s="7">
-        <v>1</v>
-      </c>
-      <c r="I19" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="13" t="s">
+      <c r="D19" s="9">
+        <v>0</v>
+      </c>
+      <c r="E19" s="15">
+        <v>1</v>
+      </c>
+      <c r="F19" s="15">
+        <v>1</v>
+      </c>
+      <c r="G19" s="15">
+        <v>1</v>
+      </c>
+      <c r="H19" s="15">
+        <v>1</v>
+      </c>
+      <c r="I19" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="22"/>
+      <c r="B20" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="9">
+        <v>5</v>
+      </c>
+      <c r="E20" s="15">
+        <v>1</v>
+      </c>
+      <c r="F20" s="15">
+        <v>1</v>
+      </c>
+      <c r="G20" s="15">
+        <v>1</v>
+      </c>
+      <c r="H20" s="15">
+        <v>1</v>
+      </c>
+      <c r="I20" s="8">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B21" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C21" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D21" s="9">
         <v>2</v>
       </c>
-      <c r="E20" s="6">
-        <v>1</v>
-      </c>
-      <c r="F20" s="6">
-        <v>1</v>
-      </c>
-      <c r="G20" s="6">
-        <v>1</v>
-      </c>
-      <c r="H20" s="6">
-        <v>0</v>
-      </c>
-      <c r="I20" s="5">
+      <c r="E21" s="9">
+        <v>1</v>
+      </c>
+      <c r="F21" s="9">
+        <v>1</v>
+      </c>
+      <c r="G21" s="9">
+        <v>1</v>
+      </c>
+      <c r="H21" s="9">
+        <v>0</v>
+      </c>
+      <c r="I21" s="8">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="14"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="5" t="s">
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="22"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="6">
-        <v>1</v>
-      </c>
-      <c r="E21" s="6">
-        <v>1</v>
-      </c>
-      <c r="F21" s="6">
-        <v>1</v>
-      </c>
-      <c r="G21" s="6">
-        <v>1</v>
-      </c>
-      <c r="H21" s="6">
-        <v>0</v>
-      </c>
-      <c r="I21" s="5">
+      <c r="D22" s="9">
+        <v>1</v>
+      </c>
+      <c r="E22" s="9">
+        <v>1</v>
+      </c>
+      <c r="F22" s="9">
+        <v>1</v>
+      </c>
+      <c r="G22" s="9">
+        <v>1</v>
+      </c>
+      <c r="H22" s="9">
+        <v>0</v>
+      </c>
+      <c r="I22" s="8">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="14"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="9" t="s">
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="22"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D23" s="9">
         <v>4</v>
       </c>
-      <c r="E22" s="6">
-        <v>1</v>
-      </c>
-      <c r="F22" s="6">
-        <v>1</v>
-      </c>
-      <c r="G22" s="6">
-        <v>1</v>
-      </c>
-      <c r="H22" s="6">
-        <v>0</v>
-      </c>
-      <c r="I22" s="5">
+      <c r="E23" s="9">
+        <v>1</v>
+      </c>
+      <c r="F23" s="9">
+        <v>1</v>
+      </c>
+      <c r="G23" s="9">
+        <v>1</v>
+      </c>
+      <c r="H23" s="9">
+        <v>0</v>
+      </c>
+      <c r="I23" s="8">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="14"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="5" t="s">
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="22"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="6">
-        <v>0</v>
-      </c>
-      <c r="E23" s="6">
-        <v>1</v>
-      </c>
-      <c r="F23" s="6">
-        <v>1</v>
-      </c>
-      <c r="G23" s="6">
-        <v>1</v>
-      </c>
-      <c r="H23" s="6">
-        <v>0</v>
-      </c>
-      <c r="I23" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="14"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="20" t="s">
+      <c r="D24" s="9">
+        <v>0</v>
+      </c>
+      <c r="E24" s="9">
+        <v>1</v>
+      </c>
+      <c r="F24" s="9">
+        <v>1</v>
+      </c>
+      <c r="G24" s="9">
+        <v>1</v>
+      </c>
+      <c r="H24" s="9">
+        <v>0</v>
+      </c>
+      <c r="I24" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="22"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="6">
-        <v>0</v>
-      </c>
-      <c r="E24" s="6">
-        <v>1</v>
-      </c>
-      <c r="F24" s="6">
-        <v>1</v>
-      </c>
-      <c r="G24" s="6">
-        <v>1</v>
-      </c>
-      <c r="H24" s="6">
-        <v>0</v>
-      </c>
-      <c r="I24" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="14"/>
-      <c r="B25" s="13" t="s">
+      <c r="D25" s="9">
+        <v>0</v>
+      </c>
+      <c r="E25" s="9">
+        <v>1</v>
+      </c>
+      <c r="F25" s="9">
+        <v>1</v>
+      </c>
+      <c r="G25" s="9">
+        <v>1</v>
+      </c>
+      <c r="H25" s="9">
+        <v>0</v>
+      </c>
+      <c r="I25" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="22"/>
+      <c r="B26" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C26" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="6">
-        <v>0</v>
-      </c>
-      <c r="E25" s="6">
-        <v>1</v>
-      </c>
-      <c r="F25" s="6">
-        <v>1</v>
-      </c>
-      <c r="G25" s="6">
-        <v>1</v>
-      </c>
-      <c r="H25" s="6">
-        <v>0</v>
-      </c>
-      <c r="I25" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="14"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="20" t="s">
+      <c r="D26" s="9">
+        <v>0</v>
+      </c>
+      <c r="E26" s="9">
+        <v>1</v>
+      </c>
+      <c r="F26" s="9">
+        <v>1</v>
+      </c>
+      <c r="G26" s="9">
+        <v>1</v>
+      </c>
+      <c r="H26" s="9">
+        <v>0</v>
+      </c>
+      <c r="I26" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="22"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="D26" s="6">
-        <v>0</v>
-      </c>
-      <c r="E26" s="6">
-        <v>1</v>
-      </c>
-      <c r="F26" s="7">
-        <v>0</v>
-      </c>
-      <c r="G26" s="6">
-        <v>1</v>
-      </c>
-      <c r="H26" s="6">
-        <v>0</v>
-      </c>
-      <c r="I26" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="14"/>
-      <c r="B27" s="13" t="s">
+      <c r="D27" s="9">
+        <v>0</v>
+      </c>
+      <c r="E27" s="9">
+        <v>1</v>
+      </c>
+      <c r="F27" s="15">
+        <v>0</v>
+      </c>
+      <c r="G27" s="9">
+        <v>1</v>
+      </c>
+      <c r="H27" s="9">
+        <v>0</v>
+      </c>
+      <c r="I27" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="22"/>
+      <c r="B28" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C28" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="6">
-        <v>0</v>
-      </c>
-      <c r="E27" s="6">
-        <v>1</v>
-      </c>
-      <c r="F27" s="6">
-        <v>1</v>
-      </c>
-      <c r="G27" s="6">
-        <v>1</v>
-      </c>
-      <c r="H27" s="6">
-        <v>0</v>
-      </c>
-      <c r="I27" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="5" t="s">
+      <c r="D28" s="9">
+        <v>0</v>
+      </c>
+      <c r="E28" s="9">
+        <v>1</v>
+      </c>
+      <c r="F28" s="9">
+        <v>1</v>
+      </c>
+      <c r="G28" s="9">
+        <v>1</v>
+      </c>
+      <c r="H28" s="9">
+        <v>0</v>
+      </c>
+      <c r="I28" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="22"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="6">
-        <v>0</v>
-      </c>
-      <c r="E28" s="6">
-        <v>1</v>
-      </c>
-      <c r="F28" s="6">
-        <v>1</v>
-      </c>
-      <c r="G28" s="6">
-        <v>1</v>
-      </c>
-      <c r="H28" s="6">
-        <v>0</v>
-      </c>
-      <c r="I28" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="13" t="s">
+      <c r="D29" s="9">
+        <v>0</v>
+      </c>
+      <c r="E29" s="9">
+        <v>1</v>
+      </c>
+      <c r="F29" s="9">
+        <v>1</v>
+      </c>
+      <c r="G29" s="9">
+        <v>1</v>
+      </c>
+      <c r="H29" s="9">
+        <v>0</v>
+      </c>
+      <c r="I29" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B30" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C30" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D30" s="9">
         <v>5</v>
       </c>
-      <c r="E29" s="6">
-        <v>1</v>
-      </c>
-      <c r="F29" s="6">
-        <v>1</v>
-      </c>
-      <c r="G29" s="6">
-        <v>1</v>
-      </c>
-      <c r="H29" s="6">
-        <v>1</v>
-      </c>
-      <c r="I29" s="5">
+      <c r="E30" s="9">
+        <v>1</v>
+      </c>
+      <c r="F30" s="9">
+        <v>1</v>
+      </c>
+      <c r="G30" s="9">
+        <v>1</v>
+      </c>
+      <c r="H30" s="9">
+        <v>1</v>
+      </c>
+      <c r="I30" s="8">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="5" t="s">
+    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="22"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D30" s="6">
-        <v>1</v>
-      </c>
-      <c r="E30" s="6">
-        <v>1</v>
-      </c>
-      <c r="F30" s="6">
-        <v>1</v>
-      </c>
-      <c r="G30" s="6">
-        <v>1</v>
-      </c>
-      <c r="H30" s="6">
-        <v>1</v>
-      </c>
-      <c r="I30" s="5">
+      <c r="D31" s="9">
+        <v>1</v>
+      </c>
+      <c r="E31" s="9">
+        <v>1</v>
+      </c>
+      <c r="F31" s="9">
+        <v>1</v>
+      </c>
+      <c r="G31" s="9">
+        <v>1</v>
+      </c>
+      <c r="H31" s="9">
+        <v>1</v>
+      </c>
+      <c r="I31" s="8">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="5" t="s">
+    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="22"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D32" s="9">
         <v>3</v>
       </c>
-      <c r="E31" s="6">
-        <v>1</v>
-      </c>
-      <c r="F31" s="6">
-        <v>1</v>
-      </c>
-      <c r="G31" s="6">
-        <v>1</v>
-      </c>
-      <c r="H31" s="6">
-        <v>1</v>
-      </c>
-      <c r="I31" s="5">
+      <c r="E32" s="9">
+        <v>1</v>
+      </c>
+      <c r="F32" s="9">
+        <v>1</v>
+      </c>
+      <c r="G32" s="9">
+        <v>1</v>
+      </c>
+      <c r="H32" s="9">
+        <v>1</v>
+      </c>
+      <c r="I32" s="8">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="13" t="s">
+    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B33" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C33" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="6">
-        <v>0</v>
-      </c>
-      <c r="E32" s="6">
-        <v>1</v>
-      </c>
-      <c r="F32" s="6">
-        <v>1</v>
-      </c>
-      <c r="G32" s="6">
-        <v>1</v>
-      </c>
-      <c r="H32" s="6">
-        <v>0</v>
-      </c>
-      <c r="I32" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="15"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="5" t="s">
+      <c r="D33" s="9">
+        <v>0</v>
+      </c>
+      <c r="E33" s="9">
+        <v>1</v>
+      </c>
+      <c r="F33" s="9">
+        <v>1</v>
+      </c>
+      <c r="G33" s="9">
+        <v>1</v>
+      </c>
+      <c r="H33" s="9">
+        <v>0</v>
+      </c>
+      <c r="I33" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="22"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D34" s="9">
         <v>4</v>
       </c>
-      <c r="E33" s="6">
-        <v>1</v>
-      </c>
-      <c r="F33" s="6">
-        <v>1</v>
-      </c>
-      <c r="G33" s="6">
-        <v>1</v>
-      </c>
-      <c r="H33" s="6">
-        <v>0</v>
-      </c>
-      <c r="I33" s="5">
+      <c r="E34" s="9">
+        <v>1</v>
+      </c>
+      <c r="F34" s="9">
+        <v>1</v>
+      </c>
+      <c r="G34" s="9">
+        <v>1</v>
+      </c>
+      <c r="H34" s="9">
+        <v>0</v>
+      </c>
+      <c r="I34" s="8">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="13" t="s">
+    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B35" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C35" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D35" s="9">
         <v>5</v>
       </c>
-      <c r="E34" s="6">
-        <v>1</v>
-      </c>
-      <c r="F34" s="6">
-        <v>1</v>
-      </c>
-      <c r="G34" s="6">
-        <v>1</v>
-      </c>
-      <c r="H34" s="6">
-        <v>0</v>
-      </c>
-      <c r="I34" s="5">
+      <c r="E35" s="9">
+        <v>1</v>
+      </c>
+      <c r="F35" s="9">
+        <v>1</v>
+      </c>
+      <c r="G35" s="9">
+        <v>1</v>
+      </c>
+      <c r="H35" s="9">
+        <v>0</v>
+      </c>
+      <c r="I35" s="8">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="5" t="s">
+    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="22"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D36" s="9">
         <v>5</v>
       </c>
-      <c r="E35" s="6">
-        <v>1</v>
-      </c>
-      <c r="F35" s="6">
-        <v>1</v>
-      </c>
-      <c r="G35" s="6">
-        <v>1</v>
-      </c>
-      <c r="H35" s="6">
-        <v>0</v>
-      </c>
-      <c r="I35" s="5">
+      <c r="E36" s="9">
+        <v>1</v>
+      </c>
+      <c r="F36" s="9">
+        <v>1</v>
+      </c>
+      <c r="G36" s="9">
+        <v>1</v>
+      </c>
+      <c r="H36" s="9">
+        <v>0</v>
+      </c>
+      <c r="I36" s="8">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="5" t="s">
+    <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="22"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D36" s="6">
-        <v>0</v>
-      </c>
-      <c r="E36" s="6">
-        <v>1</v>
-      </c>
-      <c r="F36" s="6">
-        <v>1</v>
-      </c>
-      <c r="G36" s="6">
-        <v>1</v>
-      </c>
-      <c r="H36" s="6">
-        <v>0</v>
-      </c>
-      <c r="I36" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="13" t="s">
+      <c r="D37" s="9">
+        <v>0</v>
+      </c>
+      <c r="E37" s="9">
+        <v>1</v>
+      </c>
+      <c r="F37" s="9">
+        <v>1</v>
+      </c>
+      <c r="G37" s="9">
+        <v>1</v>
+      </c>
+      <c r="H37" s="9">
+        <v>0</v>
+      </c>
+      <c r="I37" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B38" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C38" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D38" s="9">
         <v>2</v>
       </c>
-      <c r="E37" s="6">
-        <v>1</v>
-      </c>
-      <c r="F37" s="6">
-        <v>1</v>
-      </c>
-      <c r="G37" s="6">
-        <v>1</v>
-      </c>
-      <c r="H37" s="6">
-        <v>0</v>
-      </c>
-      <c r="I37" s="5">
+      <c r="E38" s="9">
+        <v>1</v>
+      </c>
+      <c r="F38" s="9">
+        <v>1</v>
+      </c>
+      <c r="G38" s="9">
+        <v>1</v>
+      </c>
+      <c r="H38" s="9">
+        <v>0</v>
+      </c>
+      <c r="I38" s="8">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="14"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="5" t="s">
+    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="22"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D39" s="9">
         <v>5</v>
       </c>
-      <c r="E38" s="6">
-        <v>1</v>
-      </c>
-      <c r="F38" s="6">
-        <v>1</v>
-      </c>
-      <c r="G38" s="6">
-        <v>1</v>
-      </c>
-      <c r="H38" s="6">
-        <v>0</v>
-      </c>
-      <c r="I38" s="5">
+      <c r="E39" s="9">
+        <v>1</v>
+      </c>
+      <c r="F39" s="9">
+        <v>1</v>
+      </c>
+      <c r="G39" s="9">
+        <v>1</v>
+      </c>
+      <c r="H39" s="9">
+        <v>0</v>
+      </c>
+      <c r="I39" s="8">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="14"/>
-      <c r="B39" s="10" t="s">
+    <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="22"/>
+      <c r="B40" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C40" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D40" s="9">
         <v>5</v>
       </c>
-      <c r="E39" s="6">
-        <v>1</v>
-      </c>
-      <c r="F39" s="6">
-        <v>1</v>
-      </c>
-      <c r="G39" s="6">
-        <v>1</v>
-      </c>
-      <c r="H39" s="6">
-        <v>0</v>
-      </c>
-      <c r="I39" s="5">
+      <c r="E40" s="9">
+        <v>1</v>
+      </c>
+      <c r="F40" s="9">
+        <v>1</v>
+      </c>
+      <c r="G40" s="9">
+        <v>1</v>
+      </c>
+      <c r="H40" s="9">
+        <v>0</v>
+      </c>
+      <c r="I40" s="8">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="14"/>
-      <c r="B40" s="10" t="s">
+    <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="22"/>
+      <c r="B41" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C41" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D41" s="9">
         <v>5</v>
       </c>
-      <c r="E40" s="6">
-        <v>1</v>
-      </c>
-      <c r="F40" s="6">
-        <v>1</v>
-      </c>
-      <c r="G40" s="6">
-        <v>1</v>
-      </c>
-      <c r="H40" s="6">
-        <v>0</v>
-      </c>
-      <c r="I40" s="5">
+      <c r="E41" s="9">
+        <v>1</v>
+      </c>
+      <c r="F41" s="9">
+        <v>1</v>
+      </c>
+      <c r="G41" s="9">
+        <v>1</v>
+      </c>
+      <c r="H41" s="9">
+        <v>0</v>
+      </c>
+      <c r="I41" s="8">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="14"/>
-      <c r="B41" s="10" t="s">
+    <row r="42" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="22"/>
+      <c r="B42" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C42" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D42" s="9">
         <v>5</v>
       </c>
-      <c r="E41" s="6">
-        <v>1</v>
-      </c>
-      <c r="F41" s="6">
-        <v>1</v>
-      </c>
-      <c r="G41" s="6">
-        <v>1</v>
-      </c>
-      <c r="H41" s="6">
-        <v>0</v>
-      </c>
-      <c r="I41" s="5">
+      <c r="E42" s="9">
+        <v>1</v>
+      </c>
+      <c r="F42" s="9">
+        <v>1</v>
+      </c>
+      <c r="G42" s="9">
+        <v>1</v>
+      </c>
+      <c r="H42" s="9">
+        <v>0</v>
+      </c>
+      <c r="I42" s="8">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="14"/>
-      <c r="B42" s="22" t="s">
+    <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="22"/>
+      <c r="B43" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="C42" s="20" t="s">
+      <c r="C43" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="D42" s="6">
-        <v>0</v>
-      </c>
-      <c r="E42" s="6">
-        <v>1</v>
-      </c>
-      <c r="F42" s="7">
-        <v>1</v>
-      </c>
-      <c r="G42" s="6">
-        <v>1</v>
-      </c>
-      <c r="H42" s="6">
-        <v>0</v>
-      </c>
-      <c r="I42" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="15"/>
-      <c r="B43" s="11" t="s">
+      <c r="D43" s="9">
+        <v>0</v>
+      </c>
+      <c r="E43" s="9">
+        <v>1</v>
+      </c>
+      <c r="F43" s="15">
+        <v>1</v>
+      </c>
+      <c r="G43" s="9">
+        <v>1</v>
+      </c>
+      <c r="H43" s="9">
+        <v>0</v>
+      </c>
+      <c r="I43" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="22"/>
+      <c r="B44" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="C44" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D44" s="9">
         <v>5</v>
       </c>
-      <c r="E43" s="6">
-        <v>1</v>
-      </c>
-      <c r="F43" s="6">
-        <v>1</v>
-      </c>
-      <c r="G43" s="6">
-        <v>1</v>
-      </c>
-      <c r="H43" s="6">
-        <v>0</v>
-      </c>
-      <c r="I43" s="5">
+      <c r="E44" s="9">
+        <v>1</v>
+      </c>
+      <c r="F44" s="9">
+        <v>1</v>
+      </c>
+      <c r="G44" s="9">
+        <v>1</v>
+      </c>
+      <c r="H44" s="9">
+        <v>0</v>
+      </c>
+      <c r="I44" s="8">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="13" t="s">
+    <row r="45" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B44" s="13" t="s">
+      <c r="B45" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C45" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D44" s="6">
-        <v>0</v>
-      </c>
-      <c r="E44" s="6">
-        <v>1</v>
-      </c>
-      <c r="F44" s="6">
-        <v>1</v>
-      </c>
-      <c r="G44" s="6">
-        <v>1</v>
-      </c>
-      <c r="H44" s="6">
-        <v>0</v>
-      </c>
-      <c r="I44" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="14"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="5" t="s">
+      <c r="D45" s="9">
+        <v>0</v>
+      </c>
+      <c r="E45" s="9">
+        <v>1</v>
+      </c>
+      <c r="F45" s="9">
+        <v>1</v>
+      </c>
+      <c r="G45" s="9">
+        <v>1</v>
+      </c>
+      <c r="H45" s="9">
+        <v>0</v>
+      </c>
+      <c r="I45" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="22"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D46" s="9">
         <v>4</v>
       </c>
-      <c r="E45" s="6">
-        <v>1</v>
-      </c>
-      <c r="F45" s="6">
-        <v>1</v>
-      </c>
-      <c r="G45" s="6">
-        <v>1</v>
-      </c>
-      <c r="H45" s="6">
-        <v>0</v>
-      </c>
-      <c r="I45" s="5">
+      <c r="E46" s="9">
+        <v>1</v>
+      </c>
+      <c r="F46" s="9">
+        <v>1</v>
+      </c>
+      <c r="G46" s="9">
+        <v>1</v>
+      </c>
+      <c r="H46" s="9">
+        <v>0</v>
+      </c>
+      <c r="I46" s="8">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="15"/>
-      <c r="B46" s="15"/>
-      <c r="C46" s="5" t="s">
+    <row r="47" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="22"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D47" s="9">
         <v>4</v>
       </c>
-      <c r="E46" s="6">
-        <v>1</v>
-      </c>
-      <c r="F46" s="6">
-        <v>1</v>
-      </c>
-      <c r="G46" s="6">
-        <v>1</v>
-      </c>
-      <c r="H46" s="6">
-        <v>0</v>
-      </c>
-      <c r="I46" s="5">
+      <c r="E47" s="9">
+        <v>1</v>
+      </c>
+      <c r="F47" s="9">
+        <v>1</v>
+      </c>
+      <c r="G47" s="9">
+        <v>1</v>
+      </c>
+      <c r="H47" s="9">
+        <v>0</v>
+      </c>
+      <c r="I47" s="8">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="H47" s="12" t="s">
+    <row r="48" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B48" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D48" s="9">
+        <v>5</v>
+      </c>
+      <c r="E48" s="9">
+        <v>1</v>
+      </c>
+      <c r="F48" s="9">
+        <v>1</v>
+      </c>
+      <c r="G48" s="9">
+        <v>1</v>
+      </c>
+      <c r="H48" s="9">
+        <v>1</v>
+      </c>
+      <c r="I48" s="8">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="22"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D49" s="9">
+        <v>5</v>
+      </c>
+      <c r="E49" s="9">
+        <v>1</v>
+      </c>
+      <c r="F49" s="9">
+        <v>1</v>
+      </c>
+      <c r="G49" s="9">
+        <v>1</v>
+      </c>
+      <c r="H49" s="9">
+        <v>1</v>
+      </c>
+      <c r="I49" s="8">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D50" s="9">
+        <v>5</v>
+      </c>
+      <c r="E50" s="9">
+        <v>1</v>
+      </c>
+      <c r="F50" s="9">
+        <v>1</v>
+      </c>
+      <c r="G50" s="9">
+        <v>1</v>
+      </c>
+      <c r="H50" s="9">
+        <v>0</v>
+      </c>
+      <c r="I50" s="8">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="22"/>
+      <c r="B51" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D51" s="12">
+        <v>4</v>
+      </c>
+      <c r="E51" s="9">
+        <v>1</v>
+      </c>
+      <c r="F51" s="9">
+        <v>0</v>
+      </c>
+      <c r="G51" s="9">
+        <v>1</v>
+      </c>
+      <c r="H51" s="9">
+        <v>0</v>
+      </c>
+      <c r="I51" s="8">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="22"/>
+      <c r="B52" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D52" s="12">
+        <v>5</v>
+      </c>
+      <c r="E52" s="9">
+        <v>0</v>
+      </c>
+      <c r="F52" s="9">
+        <v>0</v>
+      </c>
+      <c r="G52" s="9">
+        <v>0</v>
+      </c>
+      <c r="H52" s="9">
+        <v>0</v>
+      </c>
+      <c r="I52" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="22"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D53" s="12">
+        <v>5</v>
+      </c>
+      <c r="E53" s="9">
+        <v>0</v>
+      </c>
+      <c r="F53" s="9">
+        <v>0</v>
+      </c>
+      <c r="G53" s="9">
+        <v>0</v>
+      </c>
+      <c r="H53" s="9">
+        <v>0</v>
+      </c>
+      <c r="I53" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H54" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="I47">
-        <f>SUM(I2:I46)</f>
-        <v>373</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="H48" s="12" t="s">
+      <c r="I54">
+        <f>SUM(I2:I53)</f>
+        <v>456</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H55" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="I48">
-        <f>4*SUM(D2:D46)</f>
-        <v>444</v>
-      </c>
-    </row>
-    <row r="49" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="H49" s="12" t="s">
+      <c r="I55">
+        <f>4*SUM(D2:D53)</f>
+        <v>580</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H56" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I49">
-        <f>ROUND(IF(I48=0,0,I47/I48), 4)</f>
-        <v>0.84009999999999996</v>
-      </c>
-    </row>
-    <row r="50" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="51" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="H51" s="16" t="s">
+      <c r="I56">
+        <f>ROUND(IF(I55=0,0,I54/I55), 4)</f>
+        <v>0.78620000000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="58" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H58" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="I51" s="17"/>
-    </row>
-    <row r="52" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="53" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="54" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="55" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="56" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="57" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="58" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="59" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="60" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="61" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="62" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="63" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="64" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+      <c r="I58" s="25"/>
+    </row>
+    <row r="59" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="60" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="61" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="62" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="63" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="64" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4813,36 +5158,47 @@
     <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="1006" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1007" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1008" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1009" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1010" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1011" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1012" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1013" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="A2:A17"/>
+  <mergeCells count="26">
     <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B21:B25"/>
     <mergeCell ref="B8:B13"/>
-    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="H58:I58"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="B2:B7"/>
     <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A28"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A37:A43"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="A21:A29"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="A38:A44"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select 0 (false) or 1 (true)" sqref="E2:H46" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select 0 (false) or 1 (true)" sqref="E2:H53" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"0.0,1.0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="D2:D46" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="D2:D53" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"0.0,1.0,2.0,3.0,4.0,5.0"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated Evaluation Framework for Dependency Analysis Excel file
</commit_message>
<xml_diff>
--- a/Evaluation Framework for Dependency Analysis.xlsx
+++ b/Evaluation Framework for Dependency Analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/eclipse-workspace/efda/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE379113-EB43-4C4C-AAB4-766945696E86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6DC924-50EE-F448-A90E-AEF34F602B0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6880" yWindow="5160" windowWidth="33600" windowHeight="19220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="540" windowWidth="33600" windowHeight="19220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EFDA framework" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="93">
   <si>
     <t>Languages</t>
   </si>
@@ -294,6 +294,12 @@
   </si>
   <si>
     <t>With npm-shrinkwrap that has requires fields</t>
+  </si>
+  <si>
+    <t>Modules</t>
+  </si>
+  <si>
+    <t>With go.mod and go.sum</t>
   </si>
 </sst>
 </file>
@@ -375,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -420,20 +426,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -799,10 +810,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -819,8 +830,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
       <c r="C3" s="8" t="s">
         <v>12</v>
       </c>
@@ -835,8 +846,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
       <c r="C4" s="8" t="s">
         <v>13</v>
       </c>
@@ -851,8 +862,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="8" t="s">
         <v>14</v>
       </c>
@@ -867,8 +878,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="29"/>
       <c r="C6" s="8" t="s">
         <v>15</v>
       </c>
@@ -883,8 +894,8 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="8" t="s">
         <v>16</v>
       </c>
@@ -899,8 +910,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="27"/>
-      <c r="B8" s="26" t="s">
+      <c r="A8" s="29"/>
+      <c r="B8" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -917,8 +928,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="27"/>
-      <c r="B9" s="28"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="32"/>
       <c r="C9" s="8" t="s">
         <v>19</v>
       </c>
@@ -933,8 +944,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="27"/>
-      <c r="B10" s="28"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="32"/>
       <c r="C10" s="8" t="s">
         <v>20</v>
       </c>
@@ -949,8 +960,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="27"/>
-      <c r="B11" s="29"/>
+      <c r="A11" s="29"/>
+      <c r="B11" s="33"/>
       <c r="C11" s="16" t="s">
         <v>75</v>
       </c>
@@ -964,8 +975,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="27"/>
-      <c r="B12" s="29"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="33"/>
       <c r="C12" s="16" t="s">
         <v>76</v>
       </c>
@@ -979,8 +990,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="27"/>
-      <c r="B13" s="29"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="33"/>
       <c r="C13" s="16" t="s">
         <v>77</v>
       </c>
@@ -994,8 +1005,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="27"/>
-      <c r="B14" s="26" t="s">
+      <c r="A14" s="29"/>
+      <c r="B14" s="28" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="8" t="s">
@@ -1012,8 +1023,8 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="17" t="s">
         <v>23</v>
       </c>
@@ -1028,8 +1039,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="27"/>
-      <c r="B16" s="26" t="s">
+      <c r="A16" s="29"/>
+      <c r="B16" s="28" t="s">
         <v>24</v>
       </c>
       <c r="C16" s="17" t="s">
@@ -1046,8 +1057,8 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="8" t="s">
         <v>15</v>
       </c>
@@ -1062,10 +1073,10 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="28" t="s">
         <v>27</v>
       </c>
       <c r="C18" s="8" t="s">
@@ -1082,8 +1093,8 @@
       </c>
     </row>
     <row r="19" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="28"/>
+      <c r="B19" s="28"/>
       <c r="C19" s="8" t="s">
         <v>29</v>
       </c>
@@ -1097,7 +1108,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="27"/>
+      <c r="A20" s="29"/>
       <c r="B20" s="13" t="s">
         <v>83</v>
       </c>
@@ -1115,10 +1126,10 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="28" t="s">
         <v>31</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -1135,8 +1146,8 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="27"/>
-      <c r="B22" s="28"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="32"/>
       <c r="C22" s="8" t="s">
         <v>33</v>
       </c>
@@ -1151,8 +1162,8 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="27"/>
-      <c r="B23" s="28"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="32"/>
       <c r="C23" s="18" t="s">
         <v>34</v>
       </c>
@@ -1167,8 +1178,8 @@
       </c>
     </row>
     <row r="24" spans="1:9" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="27"/>
-      <c r="B24" s="28"/>
+      <c r="A24" s="29"/>
+      <c r="B24" s="32"/>
       <c r="C24" s="23" t="s">
         <v>90</v>
       </c>
@@ -1183,8 +1194,8 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="27"/>
-      <c r="B25" s="28"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="32"/>
       <c r="C25" s="8" t="s">
         <v>35</v>
       </c>
@@ -1199,8 +1210,8 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="27"/>
-      <c r="B26" s="29"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="33"/>
       <c r="C26" s="16" t="s">
         <v>72</v>
       </c>
@@ -1214,8 +1225,8 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="27"/>
-      <c r="B27" s="26" t="s">
+      <c r="A27" s="29"/>
+      <c r="B27" s="28" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="8" t="s">
@@ -1232,8 +1243,8 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="27"/>
-      <c r="B28" s="30"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="34"/>
       <c r="C28" s="16" t="s">
         <v>71</v>
       </c>
@@ -1247,8 +1258,8 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="27"/>
-      <c r="B29" s="26" t="s">
+      <c r="A29" s="29"/>
+      <c r="B29" s="28" t="s">
         <v>37</v>
       </c>
       <c r="C29" s="8" t="s">
@@ -1265,8 +1276,8 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="27"/>
-      <c r="B30" s="27"/>
+      <c r="A30" s="29"/>
+      <c r="B30" s="29"/>
       <c r="C30" s="8" t="s">
         <v>15</v>
       </c>
@@ -1281,10 +1292,10 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="26" t="s">
+      <c r="A31" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="28" t="s">
         <v>40</v>
       </c>
       <c r="C31" s="8" t="s">
@@ -1301,8 +1312,8 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="27"/>
-      <c r="B32" s="27"/>
+      <c r="A32" s="29"/>
+      <c r="B32" s="29"/>
       <c r="C32" s="8" t="s">
         <v>41</v>
       </c>
@@ -1317,8 +1328,8 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="27"/>
-      <c r="B33" s="27"/>
+      <c r="A33" s="29"/>
+      <c r="B33" s="29"/>
       <c r="C33" s="8" t="s">
         <v>42</v>
       </c>
@@ -1333,10 +1344,10 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="26" t="s">
+      <c r="A34" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="28" t="s">
         <v>44</v>
       </c>
       <c r="C34" s="8" t="s">
@@ -1353,8 +1364,8 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="27"/>
-      <c r="B35" s="27"/>
+      <c r="A35" s="29"/>
+      <c r="B35" s="29"/>
       <c r="C35" s="8" t="s">
         <v>46</v>
       </c>
@@ -1369,10 +1380,10 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="26" t="s">
+      <c r="A36" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B36" s="26" t="s">
+      <c r="B36" s="28" t="s">
         <v>48</v>
       </c>
       <c r="C36" s="8" t="s">
@@ -1389,8 +1400,8 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="27"/>
-      <c r="B37" s="27"/>
+      <c r="A37" s="29"/>
+      <c r="B37" s="29"/>
       <c r="C37" s="8" t="s">
         <v>50</v>
       </c>
@@ -1405,8 +1416,8 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="27"/>
-      <c r="B38" s="27"/>
+      <c r="A38" s="29"/>
+      <c r="B38" s="29"/>
       <c r="C38" s="8" t="s">
         <v>51</v>
       </c>
@@ -1421,10 +1432,10 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="26" t="s">
+      <c r="A39" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="B39" s="26" t="s">
+      <c r="B39" s="28" t="s">
         <v>53</v>
       </c>
       <c r="C39" s="8" t="s">
@@ -1441,8 +1452,8 @@
       </c>
     </row>
     <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="27"/>
-      <c r="B40" s="27"/>
+      <c r="A40" s="29"/>
+      <c r="B40" s="29"/>
       <c r="C40" s="8" t="s">
         <v>55</v>
       </c>
@@ -1457,7 +1468,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="27"/>
+      <c r="A41" s="29"/>
       <c r="B41" s="13" t="s">
         <v>56</v>
       </c>
@@ -1475,7 +1486,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="27"/>
+      <c r="A42" s="29"/>
       <c r="B42" s="13" t="s">
         <v>58</v>
       </c>
@@ -1493,7 +1504,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="27"/>
+      <c r="A43" s="29"/>
       <c r="B43" s="13" t="s">
         <v>60</v>
       </c>
@@ -1511,7 +1522,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="27"/>
+      <c r="A44" s="29"/>
       <c r="B44" s="19" t="s">
         <v>73</v>
       </c>
@@ -1528,7 +1539,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="27"/>
+      <c r="A45" s="29"/>
       <c r="B45" s="20" t="s">
         <v>17</v>
       </c>
@@ -1546,10 +1557,10 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="26" t="s">
+      <c r="A46" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="B46" s="26" t="s">
+      <c r="B46" s="28" t="s">
         <v>64</v>
       </c>
       <c r="C46" s="8" t="s">
@@ -1566,8 +1577,8 @@
       </c>
     </row>
     <row r="47" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="27"/>
-      <c r="B47" s="27"/>
+      <c r="A47" s="29"/>
+      <c r="B47" s="29"/>
       <c r="C47" s="8" t="s">
         <v>66</v>
       </c>
@@ -1582,8 +1593,8 @@
       </c>
     </row>
     <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="27"/>
-      <c r="B48" s="27"/>
+      <c r="A48" s="29"/>
+      <c r="B48" s="29"/>
       <c r="C48" s="8" t="s">
         <v>25</v>
       </c>
@@ -1598,10 +1609,10 @@
       </c>
     </row>
     <row r="49" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="26" t="s">
+      <c r="A49" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="B49" s="26" t="s">
+      <c r="B49" s="28" t="s">
         <v>86</v>
       </c>
       <c r="C49" s="8" t="s">
@@ -1617,8 +1628,8 @@
       </c>
     </row>
     <row r="50" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="26"/>
-      <c r="B50" s="26"/>
+      <c r="A50" s="28"/>
+      <c r="B50" s="28"/>
       <c r="C50" s="8" t="s">
         <v>88</v>
       </c>
@@ -1632,7 +1643,7 @@
       </c>
     </row>
     <row r="51" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="26" t="s">
+      <c r="A51" s="28" t="s">
         <v>78</v>
       </c>
       <c r="B51" s="14" t="s">
@@ -1651,7 +1662,7 @@
       </c>
     </row>
     <row r="52" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="26"/>
+      <c r="A52" s="28"/>
       <c r="B52" s="14" t="s">
         <v>82</v>
       </c>
@@ -1668,8 +1679,8 @@
       </c>
     </row>
     <row r="53" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="26"/>
-      <c r="B53" s="31" t="s">
+      <c r="A53" s="28"/>
+      <c r="B53" s="27" t="s">
         <v>89</v>
       </c>
       <c r="C53" s="8" t="s">
@@ -1685,8 +1696,8 @@
       </c>
     </row>
     <row r="54" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="26"/>
-      <c r="B54" s="31"/>
+      <c r="A54" s="28"/>
+      <c r="B54" s="27"/>
       <c r="C54" s="10" t="s">
         <v>81</v>
       </c>
@@ -1729,10 +1740,10 @@
     </row>
     <row r="58" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="59" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="H59" s="24" t="s">
+      <c r="H59" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="I59" s="25"/>
+      <c r="I59" s="31"/>
     </row>
     <row r="60" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="61" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2691,16 +2702,6 @@
     <row r="1014" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A39:A45"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B46:B48"/>
     <mergeCell ref="H59:I59"/>
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="B2:B7"/>
@@ -2717,6 +2718,16 @@
     <mergeCell ref="B8:B13"/>
     <mergeCell ref="B21:B26"/>
     <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A39:A45"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B46:B48"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select 0 (false) or 1 (true)" sqref="E2:H51" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -2732,10 +2743,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I1014"/>
+  <dimension ref="A1:I1015"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2781,10 +2792,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -2806,13 +2817,13 @@
         <v>1</v>
       </c>
       <c r="I2" s="8">
-        <f t="shared" ref="I2:I54" si="0">SUM(E2:H2)*D2</f>
+        <f t="shared" ref="I2:I55" si="0">SUM(E2:H2)*D2</f>
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
       <c r="C3" s="8" t="s">
         <v>12</v>
       </c>
@@ -2837,8 +2848,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="8" t="s">
         <v>13</v>
       </c>
@@ -2863,8 +2874,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="8" t="s">
         <v>14</v>
       </c>
@@ -2889,8 +2900,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
       <c r="C6" s="8" t="s">
         <v>15</v>
       </c>
@@ -2915,8 +2926,8 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="8" t="s">
         <v>16</v>
       </c>
@@ -2941,8 +2952,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26" t="s">
+      <c r="A8" s="28"/>
+      <c r="B8" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -2969,8 +2980,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="8" t="s">
         <v>19</v>
       </c>
@@ -2995,8 +3006,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="8" t="s">
         <v>20</v>
       </c>
@@ -3021,8 +3032,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="28"/>
       <c r="C11" s="16" t="s">
         <v>75</v>
       </c>
@@ -3047,8 +3058,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
       <c r="C12" s="16" t="s">
         <v>76</v>
       </c>
@@ -3073,8 +3084,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="16" t="s">
         <v>77</v>
       </c>
@@ -3099,8 +3110,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26" t="s">
+      <c r="A14" s="28"/>
+      <c r="B14" s="28" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="8" t="s">
@@ -3127,8 +3138,8 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="17" t="s">
         <v>23</v>
       </c>
@@ -3153,8 +3164,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26" t="s">
+      <c r="A16" s="28"/>
+      <c r="B16" s="28" t="s">
         <v>24</v>
       </c>
       <c r="C16" s="17" t="s">
@@ -3181,8 +3192,8 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="28"/>
       <c r="C17" s="8" t="s">
         <v>15</v>
       </c>
@@ -3207,10 +3218,10 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="28" t="s">
         <v>27</v>
       </c>
       <c r="C18" s="8" t="s">
@@ -3237,8 +3248,8 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="28"/>
+      <c r="B19" s="28"/>
       <c r="C19" s="8" t="s">
         <v>29</v>
       </c>
@@ -3263,7 +3274,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="26"/>
+      <c r="A20" s="28"/>
       <c r="B20" s="13" t="s">
         <v>83</v>
       </c>
@@ -3291,10 +3302,10 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="28" t="s">
         <v>31</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -3321,8 +3332,8 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
+      <c r="A22" s="28"/>
+      <c r="B22" s="28"/>
       <c r="C22" s="8" t="s">
         <v>33</v>
       </c>
@@ -3347,8 +3358,8 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
+      <c r="A23" s="28"/>
+      <c r="B23" s="28"/>
       <c r="C23" s="18" t="s">
         <v>34</v>
       </c>
@@ -3373,8 +3384,8 @@
       </c>
     </row>
     <row r="24" spans="1:9" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="26"/>
-      <c r="B24" s="26"/>
+      <c r="A24" s="28"/>
+      <c r="B24" s="28"/>
       <c r="C24" s="23" t="s">
         <v>90</v>
       </c>
@@ -3399,8 +3410,8 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="26"/>
-      <c r="B25" s="26"/>
+      <c r="A25" s="28"/>
+      <c r="B25" s="28"/>
       <c r="C25" s="8" t="s">
         <v>35</v>
       </c>
@@ -3425,8 +3436,8 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
+      <c r="A26" s="28"/>
+      <c r="B26" s="28"/>
       <c r="C26" s="16" t="s">
         <v>72</v>
       </c>
@@ -3451,8 +3462,8 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="26"/>
-      <c r="B27" s="26" t="s">
+      <c r="A27" s="28"/>
+      <c r="B27" s="28" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="8" t="s">
@@ -3479,8 +3490,8 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="26"/>
-      <c r="B28" s="26"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="28"/>
       <c r="C28" s="16" t="s">
         <v>71</v>
       </c>
@@ -3505,8 +3516,8 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="26"/>
-      <c r="B29" s="26" t="s">
+      <c r="A29" s="28"/>
+      <c r="B29" s="28" t="s">
         <v>37</v>
       </c>
       <c r="C29" s="8" t="s">
@@ -3533,8 +3544,8 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="26"/>
-      <c r="B30" s="26"/>
+      <c r="A30" s="28"/>
+      <c r="B30" s="28"/>
       <c r="C30" s="8" t="s">
         <v>15</v>
       </c>
@@ -3559,10 +3570,10 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="26" t="s">
+      <c r="A31" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="28" t="s">
         <v>40</v>
       </c>
       <c r="C31" s="8" t="s">
@@ -3589,8 +3600,8 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="26"/>
-      <c r="B32" s="26"/>
+      <c r="A32" s="28"/>
+      <c r="B32" s="28"/>
       <c r="C32" s="8" t="s">
         <v>41</v>
       </c>
@@ -3615,8 +3626,8 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="26"/>
-      <c r="B33" s="26"/>
+      <c r="A33" s="28"/>
+      <c r="B33" s="28"/>
       <c r="C33" s="8" t="s">
         <v>42</v>
       </c>
@@ -3641,10 +3652,10 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="26" t="s">
+      <c r="A34" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="28" t="s">
         <v>44</v>
       </c>
       <c r="C34" s="8" t="s">
@@ -3671,8 +3682,8 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="26"/>
-      <c r="B35" s="26"/>
+      <c r="A35" s="28"/>
+      <c r="B35" s="28"/>
       <c r="C35" s="8" t="s">
         <v>46</v>
       </c>
@@ -3697,10 +3708,10 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="26" t="s">
+      <c r="A36" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B36" s="26" t="s">
+      <c r="B36" s="28" t="s">
         <v>48</v>
       </c>
       <c r="C36" s="8" t="s">
@@ -3727,8 +3738,8 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="26"/>
-      <c r="B37" s="26"/>
+      <c r="A37" s="28"/>
+      <c r="B37" s="28"/>
       <c r="C37" s="8" t="s">
         <v>50</v>
       </c>
@@ -3753,8 +3764,8 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="26"/>
-      <c r="B38" s="26"/>
+      <c r="A38" s="28"/>
+      <c r="B38" s="28"/>
       <c r="C38" s="8" t="s">
         <v>51</v>
       </c>
@@ -3779,10 +3790,10 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="26" t="s">
+      <c r="A39" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="B39" s="26" t="s">
+      <c r="B39" s="28" t="s">
         <v>53</v>
       </c>
       <c r="C39" s="8" t="s">
@@ -3809,8 +3820,8 @@
       </c>
     </row>
     <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="26"/>
-      <c r="B40" s="26"/>
+      <c r="A40" s="28"/>
+      <c r="B40" s="28"/>
       <c r="C40" s="8" t="s">
         <v>55</v>
       </c>
@@ -3835,7 +3846,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="26"/>
+      <c r="A41" s="28"/>
       <c r="B41" s="13" t="s">
         <v>56</v>
       </c>
@@ -3863,7 +3874,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="26"/>
+      <c r="A42" s="28"/>
       <c r="B42" s="13" t="s">
         <v>58</v>
       </c>
@@ -3891,7 +3902,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="26"/>
+      <c r="A43" s="28"/>
       <c r="B43" s="13" t="s">
         <v>60</v>
       </c>
@@ -3919,7 +3930,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="26"/>
+      <c r="A44" s="28"/>
       <c r="B44" s="19" t="s">
         <v>73</v>
       </c>
@@ -3946,13 +3957,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="26"/>
-      <c r="B45" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C45" s="18" t="s">
-        <v>62</v>
+    <row r="45" spans="1:9" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="28"/>
+      <c r="B45" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" s="26" t="s">
+        <v>92</v>
       </c>
       <c r="D45" s="9">
         <v>5</v>
@@ -3960,81 +3971,83 @@
       <c r="E45" s="9">
         <v>1</v>
       </c>
-      <c r="F45" s="9">
+      <c r="F45" s="15">
         <v>1</v>
       </c>
       <c r="G45" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H45" s="9">
         <v>0</v>
       </c>
-      <c r="I45" s="8">
+      <c r="I45" s="26">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="28"/>
+      <c r="B46" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D46" s="9">
+        <v>5</v>
+      </c>
+      <c r="E46" s="9">
+        <v>1</v>
+      </c>
+      <c r="F46" s="9">
+        <v>1</v>
+      </c>
+      <c r="G46" s="9">
+        <v>1</v>
+      </c>
+      <c r="H46" s="9">
+        <v>0</v>
+      </c>
+      <c r="I46" s="8">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="26" t="s">
+    <row r="47" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="B46" s="26" t="s">
+      <c r="B47" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C47" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D46" s="9">
-        <v>0</v>
-      </c>
-      <c r="E46" s="9">
-        <v>1</v>
-      </c>
-      <c r="F46" s="9">
-        <v>1</v>
-      </c>
-      <c r="G46" s="9">
-        <v>1</v>
-      </c>
-      <c r="H46" s="9">
-        <v>0</v>
-      </c>
-      <c r="I46" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="26"/>
-      <c r="B47" s="26"/>
-      <c r="C47" s="8" t="s">
+      <c r="D47" s="9">
+        <v>0</v>
+      </c>
+      <c r="E47" s="9">
+        <v>1</v>
+      </c>
+      <c r="F47" s="9">
+        <v>1</v>
+      </c>
+      <c r="G47" s="9">
+        <v>1</v>
+      </c>
+      <c r="H47" s="9">
+        <v>0</v>
+      </c>
+      <c r="I47" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="28"/>
+      <c r="B48" s="28"/>
+      <c r="C48" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="D47" s="9">
-        <v>4</v>
-      </c>
-      <c r="E47" s="9">
-        <v>1</v>
-      </c>
-      <c r="F47" s="9">
-        <v>1</v>
-      </c>
-      <c r="G47" s="9">
-        <v>1</v>
-      </c>
-      <c r="H47" s="9">
-        <v>0</v>
-      </c>
-      <c r="I47" s="8">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="26"/>
-      <c r="B48" s="26"/>
-      <c r="C48" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="D48" s="9">
         <v>4</v>
@@ -4056,41 +4069,41 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="26" t="s">
+    <row r="49" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="28"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D49" s="9">
+        <v>4</v>
+      </c>
+      <c r="E49" s="9">
+        <v>1</v>
+      </c>
+      <c r="F49" s="9">
+        <v>1</v>
+      </c>
+      <c r="G49" s="9">
+        <v>1</v>
+      </c>
+      <c r="H49" s="9">
+        <v>0</v>
+      </c>
+      <c r="I49" s="8">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="B49" s="26" t="s">
+      <c r="B50" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="C49" s="8" t="s">
+      <c r="C50" s="8" t="s">
         <v>87</v>
-      </c>
-      <c r="D49" s="9">
-        <v>5</v>
-      </c>
-      <c r="E49" s="9">
-        <v>1</v>
-      </c>
-      <c r="F49" s="9">
-        <v>1</v>
-      </c>
-      <c r="G49" s="9">
-        <v>1</v>
-      </c>
-      <c r="H49" s="9">
-        <v>1</v>
-      </c>
-      <c r="I49" s="8">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="26"/>
-      <c r="B50" s="26"/>
-      <c r="C50" s="8" t="s">
-        <v>88</v>
       </c>
       <c r="D50" s="9">
         <v>5</v>
@@ -4113,14 +4126,10 @@
       </c>
     </row>
     <row r="51" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="B51" s="14" t="s">
-        <v>79</v>
-      </c>
+      <c r="A51" s="28"/>
+      <c r="B51" s="28"/>
       <c r="C51" s="8" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="D51" s="9">
         <v>5</v>
@@ -4135,29 +4144,31 @@
         <v>1</v>
       </c>
       <c r="H51" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I51" s="8">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="26"/>
+      <c r="A52" s="28" t="s">
+        <v>78</v>
+      </c>
       <c r="B52" s="14" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D52" s="12">
-        <v>4</v>
+      <c r="D52" s="9">
+        <v>5</v>
       </c>
       <c r="E52" s="9">
         <v>1</v>
       </c>
       <c r="F52" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G52" s="9">
         <v>1</v>
@@ -4167,42 +4178,44 @@
       </c>
       <c r="I52" s="8">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="53" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="26"/>
-      <c r="B53" s="31" t="s">
-        <v>89</v>
+      <c r="A53" s="28"/>
+      <c r="B53" s="14" t="s">
+        <v>82</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>80</v>
       </c>
       <c r="D53" s="12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E53" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53" s="9">
         <v>0</v>
       </c>
       <c r="G53" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H53" s="9">
         <v>0</v>
       </c>
       <c r="I53" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="26"/>
-      <c r="B54" s="31"/>
-      <c r="C54" s="10" t="s">
-        <v>81</v>
+      <c r="A54" s="28"/>
+      <c r="B54" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>80</v>
       </c>
       <c r="D54" s="12">
         <v>5</v>
@@ -4224,41 +4237,66 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="H55" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="I55">
-        <f>SUM(I2:I54)</f>
-        <v>468</v>
+    <row r="55" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="28"/>
+      <c r="B55" s="27"/>
+      <c r="C55" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D55" s="12">
+        <v>5</v>
+      </c>
+      <c r="E55" s="9">
+        <v>0</v>
+      </c>
+      <c r="F55" s="9">
+        <v>0</v>
+      </c>
+      <c r="G55" s="9">
+        <v>0</v>
+      </c>
+      <c r="H55" s="9">
+        <v>0</v>
+      </c>
+      <c r="I55" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="H56" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I56">
-        <f>4*SUM(D2:D54)</f>
-        <v>596</v>
+        <f>SUM(I2:I55)</f>
+        <v>478</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="H57" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I57">
+        <f>4*SUM(D2:D55)</f>
+        <v>616</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H58" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I57">
-        <f>ROUND(IF(I56=0,0,I55/I56), 4)</f>
-        <v>0.78520000000000001</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="59" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="H59" s="24" t="s">
+      <c r="I58">
+        <f>ROUND(IF(I57=0,0,I56/I57), 4)</f>
+        <v>0.77600000000000002</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="60" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H60" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="I59" s="25"/>
-    </row>
-    <row r="60" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+      <c r="I60" s="31"/>
+    </row>
     <row r="61" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="62" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="63" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5213,40 +5251,41 @@
     <row r="1012" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="1013" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="1014" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1015" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A39:A45"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B21:B26"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="H60:I60"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="B2:B7"/>
     <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A47:A49"/>
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="B29:B30"/>
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="B47:B49"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="A21:A30"/>
     <mergeCell ref="A31:A33"/>
     <mergeCell ref="A36:A38"/>
     <mergeCell ref="A2:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B21:B26"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="A39:A46"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:B51"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select 0 (false) or 1 (true)" sqref="E2:H54" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select 0 (false) or 1 (true)" sqref="E2:H55" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"0.0,1.0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="D2:D54" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="D2:D55" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"0.0,1.0,2.0,3.0,4.0,5.0"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Go Modules Example (#19)
Add go modules project at modulesgolang/modules/modules-basic
</commit_message>
<xml_diff>
--- a/Evaluation Framework for Dependency Analysis.xlsx
+++ b/Evaluation Framework for Dependency Analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/eclipse-workspace/efda/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE379113-EB43-4C4C-AAB4-766945696E86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6DC924-50EE-F448-A90E-AEF34F602B0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6880" yWindow="5160" windowWidth="33600" windowHeight="19220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="540" windowWidth="33600" windowHeight="19220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EFDA framework" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="93">
   <si>
     <t>Languages</t>
   </si>
@@ -294,6 +294,12 @@
   </si>
   <si>
     <t>With npm-shrinkwrap that has requires fields</t>
+  </si>
+  <si>
+    <t>Modules</t>
+  </si>
+  <si>
+    <t>With go.mod and go.sum</t>
   </si>
 </sst>
 </file>
@@ -375,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -420,20 +426,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -799,10 +810,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -819,8 +830,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
       <c r="C3" s="8" t="s">
         <v>12</v>
       </c>
@@ -835,8 +846,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
       <c r="C4" s="8" t="s">
         <v>13</v>
       </c>
@@ -851,8 +862,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="8" t="s">
         <v>14</v>
       </c>
@@ -867,8 +878,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="29"/>
       <c r="C6" s="8" t="s">
         <v>15</v>
       </c>
@@ -883,8 +894,8 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="8" t="s">
         <v>16</v>
       </c>
@@ -899,8 +910,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="27"/>
-      <c r="B8" s="26" t="s">
+      <c r="A8" s="29"/>
+      <c r="B8" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -917,8 +928,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="27"/>
-      <c r="B9" s="28"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="32"/>
       <c r="C9" s="8" t="s">
         <v>19</v>
       </c>
@@ -933,8 +944,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="27"/>
-      <c r="B10" s="28"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="32"/>
       <c r="C10" s="8" t="s">
         <v>20</v>
       </c>
@@ -949,8 +960,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="27"/>
-      <c r="B11" s="29"/>
+      <c r="A11" s="29"/>
+      <c r="B11" s="33"/>
       <c r="C11" s="16" t="s">
         <v>75</v>
       </c>
@@ -964,8 +975,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="27"/>
-      <c r="B12" s="29"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="33"/>
       <c r="C12" s="16" t="s">
         <v>76</v>
       </c>
@@ -979,8 +990,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="27"/>
-      <c r="B13" s="29"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="33"/>
       <c r="C13" s="16" t="s">
         <v>77</v>
       </c>
@@ -994,8 +1005,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="27"/>
-      <c r="B14" s="26" t="s">
+      <c r="A14" s="29"/>
+      <c r="B14" s="28" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="8" t="s">
@@ -1012,8 +1023,8 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="17" t="s">
         <v>23</v>
       </c>
@@ -1028,8 +1039,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="27"/>
-      <c r="B16" s="26" t="s">
+      <c r="A16" s="29"/>
+      <c r="B16" s="28" t="s">
         <v>24</v>
       </c>
       <c r="C16" s="17" t="s">
@@ -1046,8 +1057,8 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="8" t="s">
         <v>15</v>
       </c>
@@ -1062,10 +1073,10 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="28" t="s">
         <v>27</v>
       </c>
       <c r="C18" s="8" t="s">
@@ -1082,8 +1093,8 @@
       </c>
     </row>
     <row r="19" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="28"/>
+      <c r="B19" s="28"/>
       <c r="C19" s="8" t="s">
         <v>29</v>
       </c>
@@ -1097,7 +1108,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="27"/>
+      <c r="A20" s="29"/>
       <c r="B20" s="13" t="s">
         <v>83</v>
       </c>
@@ -1115,10 +1126,10 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="28" t="s">
         <v>31</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -1135,8 +1146,8 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="27"/>
-      <c r="B22" s="28"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="32"/>
       <c r="C22" s="8" t="s">
         <v>33</v>
       </c>
@@ -1151,8 +1162,8 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="27"/>
-      <c r="B23" s="28"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="32"/>
       <c r="C23" s="18" t="s">
         <v>34</v>
       </c>
@@ -1167,8 +1178,8 @@
       </c>
     </row>
     <row r="24" spans="1:9" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="27"/>
-      <c r="B24" s="28"/>
+      <c r="A24" s="29"/>
+      <c r="B24" s="32"/>
       <c r="C24" s="23" t="s">
         <v>90</v>
       </c>
@@ -1183,8 +1194,8 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="27"/>
-      <c r="B25" s="28"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="32"/>
       <c r="C25" s="8" t="s">
         <v>35</v>
       </c>
@@ -1199,8 +1210,8 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="27"/>
-      <c r="B26" s="29"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="33"/>
       <c r="C26" s="16" t="s">
         <v>72</v>
       </c>
@@ -1214,8 +1225,8 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="27"/>
-      <c r="B27" s="26" t="s">
+      <c r="A27" s="29"/>
+      <c r="B27" s="28" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="8" t="s">
@@ -1232,8 +1243,8 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="27"/>
-      <c r="B28" s="30"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="34"/>
       <c r="C28" s="16" t="s">
         <v>71</v>
       </c>
@@ -1247,8 +1258,8 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="27"/>
-      <c r="B29" s="26" t="s">
+      <c r="A29" s="29"/>
+      <c r="B29" s="28" t="s">
         <v>37</v>
       </c>
       <c r="C29" s="8" t="s">
@@ -1265,8 +1276,8 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="27"/>
-      <c r="B30" s="27"/>
+      <c r="A30" s="29"/>
+      <c r="B30" s="29"/>
       <c r="C30" s="8" t="s">
         <v>15</v>
       </c>
@@ -1281,10 +1292,10 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="26" t="s">
+      <c r="A31" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="28" t="s">
         <v>40</v>
       </c>
       <c r="C31" s="8" t="s">
@@ -1301,8 +1312,8 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="27"/>
-      <c r="B32" s="27"/>
+      <c r="A32" s="29"/>
+      <c r="B32" s="29"/>
       <c r="C32" s="8" t="s">
         <v>41</v>
       </c>
@@ -1317,8 +1328,8 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="27"/>
-      <c r="B33" s="27"/>
+      <c r="A33" s="29"/>
+      <c r="B33" s="29"/>
       <c r="C33" s="8" t="s">
         <v>42</v>
       </c>
@@ -1333,10 +1344,10 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="26" t="s">
+      <c r="A34" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="28" t="s">
         <v>44</v>
       </c>
       <c r="C34" s="8" t="s">
@@ -1353,8 +1364,8 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="27"/>
-      <c r="B35" s="27"/>
+      <c r="A35" s="29"/>
+      <c r="B35" s="29"/>
       <c r="C35" s="8" t="s">
         <v>46</v>
       </c>
@@ -1369,10 +1380,10 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="26" t="s">
+      <c r="A36" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B36" s="26" t="s">
+      <c r="B36" s="28" t="s">
         <v>48</v>
       </c>
       <c r="C36" s="8" t="s">
@@ -1389,8 +1400,8 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="27"/>
-      <c r="B37" s="27"/>
+      <c r="A37" s="29"/>
+      <c r="B37" s="29"/>
       <c r="C37" s="8" t="s">
         <v>50</v>
       </c>
@@ -1405,8 +1416,8 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="27"/>
-      <c r="B38" s="27"/>
+      <c r="A38" s="29"/>
+      <c r="B38" s="29"/>
       <c r="C38" s="8" t="s">
         <v>51</v>
       </c>
@@ -1421,10 +1432,10 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="26" t="s">
+      <c r="A39" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="B39" s="26" t="s">
+      <c r="B39" s="28" t="s">
         <v>53</v>
       </c>
       <c r="C39" s="8" t="s">
@@ -1441,8 +1452,8 @@
       </c>
     </row>
     <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="27"/>
-      <c r="B40" s="27"/>
+      <c r="A40" s="29"/>
+      <c r="B40" s="29"/>
       <c r="C40" s="8" t="s">
         <v>55</v>
       </c>
@@ -1457,7 +1468,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="27"/>
+      <c r="A41" s="29"/>
       <c r="B41" s="13" t="s">
         <v>56</v>
       </c>
@@ -1475,7 +1486,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="27"/>
+      <c r="A42" s="29"/>
       <c r="B42" s="13" t="s">
         <v>58</v>
       </c>
@@ -1493,7 +1504,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="27"/>
+      <c r="A43" s="29"/>
       <c r="B43" s="13" t="s">
         <v>60</v>
       </c>
@@ -1511,7 +1522,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="27"/>
+      <c r="A44" s="29"/>
       <c r="B44" s="19" t="s">
         <v>73</v>
       </c>
@@ -1528,7 +1539,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="27"/>
+      <c r="A45" s="29"/>
       <c r="B45" s="20" t="s">
         <v>17</v>
       </c>
@@ -1546,10 +1557,10 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="26" t="s">
+      <c r="A46" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="B46" s="26" t="s">
+      <c r="B46" s="28" t="s">
         <v>64</v>
       </c>
       <c r="C46" s="8" t="s">
@@ -1566,8 +1577,8 @@
       </c>
     </row>
     <row r="47" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="27"/>
-      <c r="B47" s="27"/>
+      <c r="A47" s="29"/>
+      <c r="B47" s="29"/>
       <c r="C47" s="8" t="s">
         <v>66</v>
       </c>
@@ -1582,8 +1593,8 @@
       </c>
     </row>
     <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="27"/>
-      <c r="B48" s="27"/>
+      <c r="A48" s="29"/>
+      <c r="B48" s="29"/>
       <c r="C48" s="8" t="s">
         <v>25</v>
       </c>
@@ -1598,10 +1609,10 @@
       </c>
     </row>
     <row r="49" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="26" t="s">
+      <c r="A49" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="B49" s="26" t="s">
+      <c r="B49" s="28" t="s">
         <v>86</v>
       </c>
       <c r="C49" s="8" t="s">
@@ -1617,8 +1628,8 @@
       </c>
     </row>
     <row r="50" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="26"/>
-      <c r="B50" s="26"/>
+      <c r="A50" s="28"/>
+      <c r="B50" s="28"/>
       <c r="C50" s="8" t="s">
         <v>88</v>
       </c>
@@ -1632,7 +1643,7 @@
       </c>
     </row>
     <row r="51" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="26" t="s">
+      <c r="A51" s="28" t="s">
         <v>78</v>
       </c>
       <c r="B51" s="14" t="s">
@@ -1651,7 +1662,7 @@
       </c>
     </row>
     <row r="52" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="26"/>
+      <c r="A52" s="28"/>
       <c r="B52" s="14" t="s">
         <v>82</v>
       </c>
@@ -1668,8 +1679,8 @@
       </c>
     </row>
     <row r="53" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="26"/>
-      <c r="B53" s="31" t="s">
+      <c r="A53" s="28"/>
+      <c r="B53" s="27" t="s">
         <v>89</v>
       </c>
       <c r="C53" s="8" t="s">
@@ -1685,8 +1696,8 @@
       </c>
     </row>
     <row r="54" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="26"/>
-      <c r="B54" s="31"/>
+      <c r="A54" s="28"/>
+      <c r="B54" s="27"/>
       <c r="C54" s="10" t="s">
         <v>81</v>
       </c>
@@ -1729,10 +1740,10 @@
     </row>
     <row r="58" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="59" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="H59" s="24" t="s">
+      <c r="H59" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="I59" s="25"/>
+      <c r="I59" s="31"/>
     </row>
     <row r="60" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="61" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2691,16 +2702,6 @@
     <row r="1014" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A39:A45"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B46:B48"/>
     <mergeCell ref="H59:I59"/>
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="B2:B7"/>
@@ -2717,6 +2718,16 @@
     <mergeCell ref="B8:B13"/>
     <mergeCell ref="B21:B26"/>
     <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A39:A45"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B46:B48"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select 0 (false) or 1 (true)" sqref="E2:H51" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -2732,10 +2743,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I1014"/>
+  <dimension ref="A1:I1015"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2781,10 +2792,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -2806,13 +2817,13 @@
         <v>1</v>
       </c>
       <c r="I2" s="8">
-        <f t="shared" ref="I2:I54" si="0">SUM(E2:H2)*D2</f>
+        <f t="shared" ref="I2:I55" si="0">SUM(E2:H2)*D2</f>
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
       <c r="C3" s="8" t="s">
         <v>12</v>
       </c>
@@ -2837,8 +2848,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="8" t="s">
         <v>13</v>
       </c>
@@ -2863,8 +2874,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="8" t="s">
         <v>14</v>
       </c>
@@ -2889,8 +2900,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
       <c r="C6" s="8" t="s">
         <v>15</v>
       </c>
@@ -2915,8 +2926,8 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="8" t="s">
         <v>16</v>
       </c>
@@ -2941,8 +2952,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26" t="s">
+      <c r="A8" s="28"/>
+      <c r="B8" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -2969,8 +2980,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="8" t="s">
         <v>19</v>
       </c>
@@ -2995,8 +3006,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="8" t="s">
         <v>20</v>
       </c>
@@ -3021,8 +3032,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="28"/>
       <c r="C11" s="16" t="s">
         <v>75</v>
       </c>
@@ -3047,8 +3058,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
       <c r="C12" s="16" t="s">
         <v>76</v>
       </c>
@@ -3073,8 +3084,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="16" t="s">
         <v>77</v>
       </c>
@@ -3099,8 +3110,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26" t="s">
+      <c r="A14" s="28"/>
+      <c r="B14" s="28" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="8" t="s">
@@ -3127,8 +3138,8 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="17" t="s">
         <v>23</v>
       </c>
@@ -3153,8 +3164,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26" t="s">
+      <c r="A16" s="28"/>
+      <c r="B16" s="28" t="s">
         <v>24</v>
       </c>
       <c r="C16" s="17" t="s">
@@ -3181,8 +3192,8 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="28"/>
       <c r="C17" s="8" t="s">
         <v>15</v>
       </c>
@@ -3207,10 +3218,10 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="28" t="s">
         <v>27</v>
       </c>
       <c r="C18" s="8" t="s">
@@ -3237,8 +3248,8 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="28"/>
+      <c r="B19" s="28"/>
       <c r="C19" s="8" t="s">
         <v>29</v>
       </c>
@@ -3263,7 +3274,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="26"/>
+      <c r="A20" s="28"/>
       <c r="B20" s="13" t="s">
         <v>83</v>
       </c>
@@ -3291,10 +3302,10 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="28" t="s">
         <v>31</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -3321,8 +3332,8 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
+      <c r="A22" s="28"/>
+      <c r="B22" s="28"/>
       <c r="C22" s="8" t="s">
         <v>33</v>
       </c>
@@ -3347,8 +3358,8 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
+      <c r="A23" s="28"/>
+      <c r="B23" s="28"/>
       <c r="C23" s="18" t="s">
         <v>34</v>
       </c>
@@ -3373,8 +3384,8 @@
       </c>
     </row>
     <row r="24" spans="1:9" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="26"/>
-      <c r="B24" s="26"/>
+      <c r="A24" s="28"/>
+      <c r="B24" s="28"/>
       <c r="C24" s="23" t="s">
         <v>90</v>
       </c>
@@ -3399,8 +3410,8 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="26"/>
-      <c r="B25" s="26"/>
+      <c r="A25" s="28"/>
+      <c r="B25" s="28"/>
       <c r="C25" s="8" t="s">
         <v>35</v>
       </c>
@@ -3425,8 +3436,8 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
+      <c r="A26" s="28"/>
+      <c r="B26" s="28"/>
       <c r="C26" s="16" t="s">
         <v>72</v>
       </c>
@@ -3451,8 +3462,8 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="26"/>
-      <c r="B27" s="26" t="s">
+      <c r="A27" s="28"/>
+      <c r="B27" s="28" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="8" t="s">
@@ -3479,8 +3490,8 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="26"/>
-      <c r="B28" s="26"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="28"/>
       <c r="C28" s="16" t="s">
         <v>71</v>
       </c>
@@ -3505,8 +3516,8 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="26"/>
-      <c r="B29" s="26" t="s">
+      <c r="A29" s="28"/>
+      <c r="B29" s="28" t="s">
         <v>37</v>
       </c>
       <c r="C29" s="8" t="s">
@@ -3533,8 +3544,8 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="26"/>
-      <c r="B30" s="26"/>
+      <c r="A30" s="28"/>
+      <c r="B30" s="28"/>
       <c r="C30" s="8" t="s">
         <v>15</v>
       </c>
@@ -3559,10 +3570,10 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="26" t="s">
+      <c r="A31" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="28" t="s">
         <v>40</v>
       </c>
       <c r="C31" s="8" t="s">
@@ -3589,8 +3600,8 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="26"/>
-      <c r="B32" s="26"/>
+      <c r="A32" s="28"/>
+      <c r="B32" s="28"/>
       <c r="C32" s="8" t="s">
         <v>41</v>
       </c>
@@ -3615,8 +3626,8 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="26"/>
-      <c r="B33" s="26"/>
+      <c r="A33" s="28"/>
+      <c r="B33" s="28"/>
       <c r="C33" s="8" t="s">
         <v>42</v>
       </c>
@@ -3641,10 +3652,10 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="26" t="s">
+      <c r="A34" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="28" t="s">
         <v>44</v>
       </c>
       <c r="C34" s="8" t="s">
@@ -3671,8 +3682,8 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="26"/>
-      <c r="B35" s="26"/>
+      <c r="A35" s="28"/>
+      <c r="B35" s="28"/>
       <c r="C35" s="8" t="s">
         <v>46</v>
       </c>
@@ -3697,10 +3708,10 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="26" t="s">
+      <c r="A36" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B36" s="26" t="s">
+      <c r="B36" s="28" t="s">
         <v>48</v>
       </c>
       <c r="C36" s="8" t="s">
@@ -3727,8 +3738,8 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="26"/>
-      <c r="B37" s="26"/>
+      <c r="A37" s="28"/>
+      <c r="B37" s="28"/>
       <c r="C37" s="8" t="s">
         <v>50</v>
       </c>
@@ -3753,8 +3764,8 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="26"/>
-      <c r="B38" s="26"/>
+      <c r="A38" s="28"/>
+      <c r="B38" s="28"/>
       <c r="C38" s="8" t="s">
         <v>51</v>
       </c>
@@ -3779,10 +3790,10 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="26" t="s">
+      <c r="A39" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="B39" s="26" t="s">
+      <c r="B39" s="28" t="s">
         <v>53</v>
       </c>
       <c r="C39" s="8" t="s">
@@ -3809,8 +3820,8 @@
       </c>
     </row>
     <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="26"/>
-      <c r="B40" s="26"/>
+      <c r="A40" s="28"/>
+      <c r="B40" s="28"/>
       <c r="C40" s="8" t="s">
         <v>55</v>
       </c>
@@ -3835,7 +3846,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="26"/>
+      <c r="A41" s="28"/>
       <c r="B41" s="13" t="s">
         <v>56</v>
       </c>
@@ -3863,7 +3874,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="26"/>
+      <c r="A42" s="28"/>
       <c r="B42" s="13" t="s">
         <v>58</v>
       </c>
@@ -3891,7 +3902,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="26"/>
+      <c r="A43" s="28"/>
       <c r="B43" s="13" t="s">
         <v>60</v>
       </c>
@@ -3919,7 +3930,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="26"/>
+      <c r="A44" s="28"/>
       <c r="B44" s="19" t="s">
         <v>73</v>
       </c>
@@ -3946,13 +3957,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="26"/>
-      <c r="B45" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C45" s="18" t="s">
-        <v>62</v>
+    <row r="45" spans="1:9" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="28"/>
+      <c r="B45" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" s="26" t="s">
+        <v>92</v>
       </c>
       <c r="D45" s="9">
         <v>5</v>
@@ -3960,81 +3971,83 @@
       <c r="E45" s="9">
         <v>1</v>
       </c>
-      <c r="F45" s="9">
+      <c r="F45" s="15">
         <v>1</v>
       </c>
       <c r="G45" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H45" s="9">
         <v>0</v>
       </c>
-      <c r="I45" s="8">
+      <c r="I45" s="26">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="28"/>
+      <c r="B46" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D46" s="9">
+        <v>5</v>
+      </c>
+      <c r="E46" s="9">
+        <v>1</v>
+      </c>
+      <c r="F46" s="9">
+        <v>1</v>
+      </c>
+      <c r="G46" s="9">
+        <v>1</v>
+      </c>
+      <c r="H46" s="9">
+        <v>0</v>
+      </c>
+      <c r="I46" s="8">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="26" t="s">
+    <row r="47" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="B46" s="26" t="s">
+      <c r="B47" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C47" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D46" s="9">
-        <v>0</v>
-      </c>
-      <c r="E46" s="9">
-        <v>1</v>
-      </c>
-      <c r="F46" s="9">
-        <v>1</v>
-      </c>
-      <c r="G46" s="9">
-        <v>1</v>
-      </c>
-      <c r="H46" s="9">
-        <v>0</v>
-      </c>
-      <c r="I46" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="26"/>
-      <c r="B47" s="26"/>
-      <c r="C47" s="8" t="s">
+      <c r="D47" s="9">
+        <v>0</v>
+      </c>
+      <c r="E47" s="9">
+        <v>1</v>
+      </c>
+      <c r="F47" s="9">
+        <v>1</v>
+      </c>
+      <c r="G47" s="9">
+        <v>1</v>
+      </c>
+      <c r="H47" s="9">
+        <v>0</v>
+      </c>
+      <c r="I47" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="28"/>
+      <c r="B48" s="28"/>
+      <c r="C48" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="D47" s="9">
-        <v>4</v>
-      </c>
-      <c r="E47" s="9">
-        <v>1</v>
-      </c>
-      <c r="F47" s="9">
-        <v>1</v>
-      </c>
-      <c r="G47" s="9">
-        <v>1</v>
-      </c>
-      <c r="H47" s="9">
-        <v>0</v>
-      </c>
-      <c r="I47" s="8">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="26"/>
-      <c r="B48" s="26"/>
-      <c r="C48" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="D48" s="9">
         <v>4</v>
@@ -4056,41 +4069,41 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="26" t="s">
+    <row r="49" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="28"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D49" s="9">
+        <v>4</v>
+      </c>
+      <c r="E49" s="9">
+        <v>1</v>
+      </c>
+      <c r="F49" s="9">
+        <v>1</v>
+      </c>
+      <c r="G49" s="9">
+        <v>1</v>
+      </c>
+      <c r="H49" s="9">
+        <v>0</v>
+      </c>
+      <c r="I49" s="8">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="B49" s="26" t="s">
+      <c r="B50" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="C49" s="8" t="s">
+      <c r="C50" s="8" t="s">
         <v>87</v>
-      </c>
-      <c r="D49" s="9">
-        <v>5</v>
-      </c>
-      <c r="E49" s="9">
-        <v>1</v>
-      </c>
-      <c r="F49" s="9">
-        <v>1</v>
-      </c>
-      <c r="G49" s="9">
-        <v>1</v>
-      </c>
-      <c r="H49" s="9">
-        <v>1</v>
-      </c>
-      <c r="I49" s="8">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="26"/>
-      <c r="B50" s="26"/>
-      <c r="C50" s="8" t="s">
-        <v>88</v>
       </c>
       <c r="D50" s="9">
         <v>5</v>
@@ -4113,14 +4126,10 @@
       </c>
     </row>
     <row r="51" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="B51" s="14" t="s">
-        <v>79</v>
-      </c>
+      <c r="A51" s="28"/>
+      <c r="B51" s="28"/>
       <c r="C51" s="8" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="D51" s="9">
         <v>5</v>
@@ -4135,29 +4144,31 @@
         <v>1</v>
       </c>
       <c r="H51" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I51" s="8">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="26"/>
+      <c r="A52" s="28" t="s">
+        <v>78</v>
+      </c>
       <c r="B52" s="14" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D52" s="12">
-        <v>4</v>
+      <c r="D52" s="9">
+        <v>5</v>
       </c>
       <c r="E52" s="9">
         <v>1</v>
       </c>
       <c r="F52" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G52" s="9">
         <v>1</v>
@@ -4167,42 +4178,44 @@
       </c>
       <c r="I52" s="8">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="53" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="26"/>
-      <c r="B53" s="31" t="s">
-        <v>89</v>
+      <c r="A53" s="28"/>
+      <c r="B53" s="14" t="s">
+        <v>82</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>80</v>
       </c>
       <c r="D53" s="12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E53" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53" s="9">
         <v>0</v>
       </c>
       <c r="G53" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H53" s="9">
         <v>0</v>
       </c>
       <c r="I53" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="26"/>
-      <c r="B54" s="31"/>
-      <c r="C54" s="10" t="s">
-        <v>81</v>
+      <c r="A54" s="28"/>
+      <c r="B54" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>80</v>
       </c>
       <c r="D54" s="12">
         <v>5</v>
@@ -4224,41 +4237,66 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="H55" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="I55">
-        <f>SUM(I2:I54)</f>
-        <v>468</v>
+    <row r="55" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="28"/>
+      <c r="B55" s="27"/>
+      <c r="C55" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D55" s="12">
+        <v>5</v>
+      </c>
+      <c r="E55" s="9">
+        <v>0</v>
+      </c>
+      <c r="F55" s="9">
+        <v>0</v>
+      </c>
+      <c r="G55" s="9">
+        <v>0</v>
+      </c>
+      <c r="H55" s="9">
+        <v>0</v>
+      </c>
+      <c r="I55" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="H56" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I56">
-        <f>4*SUM(D2:D54)</f>
-        <v>596</v>
+        <f>SUM(I2:I55)</f>
+        <v>478</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="H57" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I57">
+        <f>4*SUM(D2:D55)</f>
+        <v>616</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H58" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I57">
-        <f>ROUND(IF(I56=0,0,I55/I56), 4)</f>
-        <v>0.78520000000000001</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="59" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="H59" s="24" t="s">
+      <c r="I58">
+        <f>ROUND(IF(I57=0,0,I56/I57), 4)</f>
+        <v>0.77600000000000002</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="60" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H60" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="I59" s="25"/>
-    </row>
-    <row r="60" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+      <c r="I60" s="31"/>
+    </row>
     <row r="61" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="62" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="63" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5213,40 +5251,41 @@
     <row r="1012" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="1013" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="1014" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1015" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A39:A45"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B21:B26"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="H60:I60"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="B2:B7"/>
     <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A47:A49"/>
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="B29:B30"/>
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="B47:B49"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="A21:A30"/>
     <mergeCell ref="A31:A33"/>
     <mergeCell ref="A36:A38"/>
     <mergeCell ref="A2:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B21:B26"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="A39:A46"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:B51"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select 0 (false) or 1 (true)" sqref="E2:H54" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select 0 (false) or 1 (true)" sqref="E2:H55" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"0.0,1.0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="D2:D54" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="D2:D55" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"0.0,1.0,2.0,3.0,4.0,5.0"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>